<commit_message>
New files from Jeff.
</commit_message>
<xml_diff>
--- a/OptFramework/Sim-energy-analysis-project-plan.xlsx
+++ b/OptFramework/Sim-energy-analysis-project-plan.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="6630" windowWidth="18195" windowHeight="6000"/>
+    <workbookView xWindow="0" yWindow="6630" windowWidth="19155" windowHeight="6000" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Planning" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="83">
   <si>
     <t>Archetype for Manatoba</t>
   </si>
@@ -241,22 +241,31 @@
     <t>PV (5 kw facing south)</t>
   </si>
   <si>
-    <t>Exterior Insulation</t>
-  </si>
-  <si>
     <t>Advanced Framing</t>
   </si>
   <si>
     <t>Exterior Foundation</t>
   </si>
   <si>
-    <t>Partial</t>
-  </si>
-  <si>
     <t>Base case (Alex)</t>
   </si>
   <si>
     <t>Base case (Jeff)</t>
+  </si>
+  <si>
+    <t>Using Jeff's base</t>
+  </si>
+  <si>
+    <t>Exterior Insulation 2" MWB</t>
+  </si>
+  <si>
+    <t>Exterior Insulation 1.5" XPS</t>
+  </si>
+  <si>
+    <t>Exterior Insulation 2.5" XPS</t>
+  </si>
+  <si>
+    <t>Patric</t>
   </si>
 </sst>
 </file>
@@ -388,7 +397,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -404,9 +413,6 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -416,6 +422,11 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="1" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -792,17 +803,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:I41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="7" topLeftCell="C8" activePane="bottomRight" state="frozenSplit"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="2" ySplit="7" topLeftCell="C23" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="F35" sqref="F35"/>
+      <selection pane="bottomRight" activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.85546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="24.5703125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="26.42578125" style="1" customWidth="1"/>
     <col min="3" max="3" width="35.140625" style="1" customWidth="1"/>
     <col min="4" max="4" width="46.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15" style="1" bestFit="1" customWidth="1"/>
@@ -1151,7 +1162,7 @@
         <v>2</v>
       </c>
       <c r="G29" s="6" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="H29" s="6"/>
       <c r="I29" s="6"/>
@@ -1168,10 +1179,10 @@
       </c>
       <c r="E30" s="5"/>
       <c r="F30" s="5" t="s">
-        <v>2</v>
+        <v>82</v>
       </c>
       <c r="G30" s="5" t="s">
-        <v>77</v>
+        <v>10</v>
       </c>
       <c r="H30" s="5"/>
       <c r="I30" s="5" t="s">
@@ -1187,11 +1198,9 @@
       <c r="E31" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="F31" s="6" t="s">
-        <v>2</v>
-      </c>
+      <c r="F31" s="6"/>
       <c r="G31" s="6" t="s">
-        <v>77</v>
+        <v>10</v>
       </c>
       <c r="H31" s="6"/>
       <c r="I31" s="6"/>
@@ -1409,21 +1418,23 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C4:H18"/>
+  <dimension ref="C4:H19"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="9.140625" style="1"/>
-    <col min="3" max="3" width="22.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="2.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="27.28515625" style="1" customWidth="1"/>
     <col min="4" max="4" width="15.7109375" style="1" customWidth="1"/>
     <col min="5" max="5" width="18.28515625" style="1" customWidth="1"/>
     <col min="6" max="6" width="19.7109375" style="1" customWidth="1"/>
     <col min="7" max="7" width="12.7109375" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="1"/>
+    <col min="8" max="8" width="15.140625" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="4" spans="3:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -1434,65 +1445,67 @@
       <c r="G4" s="2"/>
     </row>
     <row r="5" spans="3:8" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C5" s="16" t="s">
+      <c r="C5" s="15" t="s">
         <v>68</v>
       </c>
-      <c r="D5" s="17" t="s">
+      <c r="D5" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="E5" s="17" t="s">
+      <c r="E5" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="F5" s="17" t="s">
+      <c r="F5" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="G5" s="17" t="s">
+      <c r="G5" s="16" t="s">
         <v>72</v>
       </c>
-      <c r="H5" s="15"/>
+      <c r="H5" s="24" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="6" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C6" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="D6" s="19">
+        <v>76</v>
+      </c>
+      <c r="D6" s="18">
         <v>12504.023999999999</v>
       </c>
-      <c r="E6" s="19">
+      <c r="E6" s="18">
         <v>2341.5479999999998</v>
       </c>
-      <c r="F6" s="18"/>
-      <c r="G6" s="18"/>
+      <c r="F6" s="17"/>
+      <c r="G6" s="17"/>
     </row>
     <row r="7" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C7" s="20" t="s">
-        <v>79</v>
-      </c>
-      <c r="D7" s="21">
-        <v>13213.58</v>
-      </c>
-      <c r="E7" s="21">
-        <v>2207.52</v>
-      </c>
-      <c r="F7" s="22"/>
-      <c r="G7" s="22"/>
+      <c r="C7" s="19" t="s">
+        <v>77</v>
+      </c>
+      <c r="D7" s="20">
+        <v>12393.647999999999</v>
+      </c>
+      <c r="E7" s="20">
+        <v>2333.6640000000002</v>
+      </c>
+      <c r="F7" s="21"/>
+      <c r="G7" s="21"/>
     </row>
     <row r="8" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C8" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D8" s="19">
+      <c r="D8" s="18">
         <v>11967.12</v>
       </c>
-      <c r="E8" s="19">
+      <c r="E8" s="18">
         <f>E6</f>
         <v>2341.5479999999998</v>
       </c>
-      <c r="F8" s="1">
+      <c r="F8" s="18">
         <f>$D$6-D8</f>
         <v>536.90399999999863</v>
       </c>
-      <c r="G8" s="1">
+      <c r="G8" s="18">
         <f>$E$6-E8</f>
         <v>0</v>
       </c>
@@ -1501,51 +1514,156 @@
       <c r="C9" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="D9" s="19">
+      <c r="D9" s="18">
         <f>D6-4.60476*5*1000*1000/3600</f>
         <v>6108.5239999999994</v>
       </c>
-      <c r="E9" s="19">
+      <c r="E9" s="18">
         <f>E6</f>
         <v>2341.5479999999998</v>
       </c>
-      <c r="F9" s="19">
+      <c r="F9" s="18">
         <f>$D$6-D9</f>
         <v>6395.5</v>
       </c>
-      <c r="G9" s="1">
+      <c r="G9" s="18">
         <f>$E$6-E9</f>
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C10" s="1" t="s">
-        <v>74</v>
+        <v>80</v>
+      </c>
+      <c r="D10" s="18">
+        <v>12362.111999999999</v>
+      </c>
+      <c r="E10" s="18">
+        <v>2144.4479999999999</v>
+      </c>
+      <c r="F10" s="18">
+        <f>IF(D10&gt;0,$D$7-D10,"")</f>
+        <v>31.536000000000058</v>
+      </c>
+      <c r="G10" s="18">
+        <f>IF(E10&gt;0,$E$7-E10,"")</f>
+        <v>189.21600000000035</v>
+      </c>
+      <c r="H10" s="19" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="11" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C11" s="1" t="s">
-        <v>75</v>
+        <v>81</v>
+      </c>
+      <c r="D11" s="18">
+        <v>12362.111999999999</v>
+      </c>
+      <c r="E11" s="18">
+        <v>2049.84</v>
+      </c>
+      <c r="F11" s="18">
+        <f>IF(D11&gt;0,$D$7-D11,"")</f>
+        <v>31.536000000000058</v>
+      </c>
+      <c r="G11" s="18">
+        <f>IF(E11&gt;0,$E$7-E11,"")</f>
+        <v>283.82400000000007</v>
+      </c>
+      <c r="H11" s="19" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="12" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C12" s="1" t="s">
-        <v>76</v>
-      </c>
+        <v>79</v>
+      </c>
+      <c r="D12" s="18"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="18" t="str">
+        <f>IF(D12&gt;0,$D$7-D12, "")</f>
+        <v/>
+      </c>
+      <c r="G12" s="18" t="str">
+        <f>IF(E12&gt;0,$E$7-E12,"")</f>
+        <v/>
+      </c>
+      <c r="H12" s="19" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="13" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C13" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D13" s="18">
+        <v>12393.647999999999</v>
+      </c>
+      <c r="E13" s="18">
+        <v>2333.6640000000002</v>
+      </c>
+      <c r="F13" s="18">
+        <f t="shared" ref="F13:F14" si="0">IF(D13&gt;0,$D$7-D13, "")</f>
+        <v>0</v>
+      </c>
+      <c r="G13" s="18">
+        <f t="shared" ref="G13:G14" si="1">IF(E13&gt;0,$E$7-E13,"")</f>
+        <v>0</v>
+      </c>
+      <c r="H13" s="19" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="14" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C14" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D14" s="18"/>
+      <c r="E14" s="18"/>
+      <c r="F14" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="G14" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="H14" s="19" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="15" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="D15" s="18"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="18"/>
+    </row>
+    <row r="16" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="D16" s="18"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="18"/>
     </row>
     <row r="17" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
-    </row>
-    <row r="18" spans="3:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="18"/>
+    </row>
+    <row r="18" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C18" s="5"/>
+      <c r="D18" s="22"/>
+      <c r="E18" s="22"/>
+      <c r="F18" s="22"/>
+      <c r="G18" s="22"/>
+    </row>
+    <row r="19" spans="3:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C19" s="2"/>
+      <c r="D19" s="23"/>
+      <c r="E19" s="23"/>
+      <c r="F19" s="23"/>
+      <c r="G19" s="23"/>
     </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>

</xml_diff>

<commit_message>
Final changes for Jeff's portion of MB LEEP runs: - updated cost in OPTIONS-General.options - updates to materials&constructions.xls - added 2.0" XPS walls to NZEH-CEF.constrdb - Final results in Sim-energy-analysis-project-plan.xlsx
</commit_message>
<xml_diff>
--- a/OptFramework/Sim-energy-analysis-project-plan.xlsx
+++ b/OptFramework/Sim-energy-analysis-project-plan.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="6630" windowWidth="19155" windowHeight="6000" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="6690" windowWidth="19155" windowHeight="5940" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Planning" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="83">
   <si>
     <t>Archetype for Manatoba</t>
   </si>
@@ -253,19 +253,19 @@
     <t>Base case (Jeff)</t>
   </si>
   <si>
-    <t>Using Jeff's base</t>
-  </si>
-  <si>
     <t>Exterior Insulation 2" MWB</t>
   </si>
   <si>
-    <t>Exterior Insulation 1.5" XPS</t>
-  </si>
-  <si>
-    <t>Exterior Insulation 2.5" XPS</t>
-  </si>
-  <si>
     <t>Patric</t>
+  </si>
+  <si>
+    <t>Exterior Insulation 2" XPS</t>
+  </si>
+  <si>
+    <t>Using Jeff's Base</t>
+  </si>
+  <si>
+    <t>Using Jeff's Base, energy results for 2" XPS</t>
   </si>
 </sst>
 </file>
@@ -422,11 +422,11 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="1" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="1" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1179,7 +1179,7 @@
       </c>
       <c r="E30" s="5"/>
       <c r="F30" s="5" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="G30" s="5" t="s">
         <v>10</v>
@@ -1418,10 +1418,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C4:H19"/>
+  <dimension ref="C4:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1460,7 +1460,7 @@
       <c r="G5" s="16" t="s">
         <v>72</v>
       </c>
-      <c r="H5" s="24" t="s">
+      <c r="H5" s="23" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1482,10 +1482,10 @@
         <v>77</v>
       </c>
       <c r="D7" s="20">
-        <v>12393.647999999999</v>
+        <v>12535.56</v>
       </c>
       <c r="E7" s="20">
-        <v>2333.6640000000002</v>
+        <v>2404.62</v>
       </c>
       <c r="F7" s="21"/>
       <c r="G7" s="21"/>
@@ -1530,136 +1530,95 @@
         <f>$E$6-E9</f>
         <v>0</v>
       </c>
+      <c r="H9" s="19"/>
     </row>
     <row r="10" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C10" s="1" t="s">
         <v>80</v>
       </c>
       <c r="D10" s="18">
-        <v>12362.111999999999</v>
+        <v>12472.487999999999</v>
       </c>
       <c r="E10" s="18">
         <v>2144.4479999999999</v>
       </c>
       <c r="F10" s="18">
         <f>IF(D10&gt;0,$D$7-D10,"")</f>
-        <v>31.536000000000058</v>
+        <v>63.072000000000116</v>
       </c>
       <c r="G10" s="18">
         <f>IF(E10&gt;0,$E$7-E10,"")</f>
-        <v>189.21600000000035</v>
+        <v>260.17200000000003</v>
       </c>
       <c r="H10" s="19" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
     </row>
     <row r="11" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C11" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D11" s="18">
-        <v>12362.111999999999</v>
+        <v>12472.487999999999</v>
       </c>
       <c r="E11" s="18">
-        <v>2049.84</v>
+        <v>2144.4479999999999</v>
       </c>
       <c r="F11" s="18">
-        <f>IF(D11&gt;0,$D$7-D11,"")</f>
-        <v>31.536000000000058</v>
+        <f>IF(D11&gt;0,$D$7-D11, "")</f>
+        <v>63.072000000000116</v>
       </c>
       <c r="G11" s="18">
         <f>IF(E11&gt;0,$E$7-E11,"")</f>
-        <v>283.82400000000007</v>
+        <v>260.17200000000003</v>
       </c>
       <c r="H11" s="19" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
     </row>
     <row r="12" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C12" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="D12" s="18"/>
-      <c r="E12" s="18"/>
-      <c r="F12" s="18" t="str">
-        <f>IF(D12&gt;0,$D$7-D12, "")</f>
-        <v/>
-      </c>
-      <c r="G12" s="18" t="str">
-        <f>IF(E12&gt;0,$E$7-E12,"")</f>
-        <v/>
+        <v>74</v>
+      </c>
+      <c r="D12" s="18">
+        <v>12535.56</v>
+      </c>
+      <c r="E12" s="18">
+        <v>2373.0839999999998</v>
+      </c>
+      <c r="F12" s="18">
+        <f t="shared" ref="F12:F13" si="0">IF(D12&gt;0,$D$7-D12, "")</f>
+        <v>0</v>
+      </c>
+      <c r="G12" s="18">
+        <f t="shared" ref="G12:G13" si="1">IF(E12&gt;0,$E$7-E12,"")</f>
+        <v>31.536000000000058</v>
       </c>
       <c r="H12" s="19" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="13" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C13" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="D13" s="18"/>
-      <c r="E13" s="18"/>
-      <c r="F13" s="18" t="str">
-        <f t="shared" ref="F13:F14" si="0">IF(D13&gt;0,$D$7-D13, "")</f>
-        <v/>
-      </c>
-      <c r="G13" s="18" t="str">
-        <f t="shared" ref="G13:G14" si="1">IF(E13&gt;0,$E$7-E13,"")</f>
-        <v/>
-      </c>
-      <c r="H13" s="19" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="14" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C14" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="13" spans="3:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C13" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="D14" s="18"/>
-      <c r="E14" s="18"/>
-      <c r="F14" s="18" t="str">
+      <c r="D13" s="22">
+        <v>12504.023999999999</v>
+      </c>
+      <c r="E13" s="22">
+        <v>2310.0120000000002</v>
+      </c>
+      <c r="F13" s="22">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="G14" s="18" t="str">
+        <v>31.536000000000058</v>
+      </c>
+      <c r="G13" s="22">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="H14" s="19" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="15" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="D15" s="18"/>
-      <c r="E15" s="18"/>
-      <c r="F15" s="18"/>
-      <c r="G15" s="18"/>
-    </row>
-    <row r="16" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="D16" s="18"/>
-      <c r="E16" s="18"/>
-      <c r="F16" s="18"/>
-      <c r="G16" s="18"/>
-    </row>
-    <row r="17" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="D17" s="18"/>
-      <c r="E17" s="18"/>
-      <c r="F17" s="18"/>
-      <c r="G17" s="18"/>
-    </row>
-    <row r="18" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C18" s="5"/>
-      <c r="D18" s="22"/>
-      <c r="E18" s="22"/>
-      <c r="F18" s="22"/>
-      <c r="G18" s="22"/>
-    </row>
-    <row r="19" spans="3:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C19" s="2"/>
-      <c r="D19" s="23"/>
-      <c r="E19" s="23"/>
-      <c r="F19" s="23"/>
-      <c r="G19" s="23"/>
+        <v>94.60799999999972</v>
+      </c>
+      <c r="H13" s="24" t="s">
+        <v>81</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>

</xml_diff>

<commit_message>
New choice files for windows, hrv, passive solar, instand DHW. Also, updated energy analysis.
</commit_message>
<xml_diff>
--- a/OptFramework/Sim-energy-analysis-project-plan.xlsx
+++ b/OptFramework/Sim-energy-analysis-project-plan.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="98">
   <si>
     <t>Archetype for Manatoba</t>
   </si>
@@ -250,29 +250,77 @@
     <t>Base case (Alex)</t>
   </si>
   <si>
-    <t>Base case (Jeff)</t>
-  </si>
-  <si>
-    <t>Exterior Insulation 2" MWB</t>
-  </si>
-  <si>
     <t>Patric</t>
   </si>
   <si>
-    <t>Exterior Insulation 2" XPS</t>
-  </si>
-  <si>
-    <t>Using Jeff's Base</t>
-  </si>
-  <si>
-    <t>Using Jeff's Base, energy results for 2" XPS</t>
+    <t>Advanced windows</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Exterior Insulation: </t>
+  </si>
+  <si>
+    <t>1.5"</t>
+  </si>
+  <si>
+    <t>2.0"</t>
+  </si>
+  <si>
+    <t>2.5"</t>
+  </si>
+  <si>
+    <t>Passive Solar</t>
+  </si>
+  <si>
+    <t>Or: south</t>
+  </si>
+  <si>
+    <t>Gas instantaneous</t>
+  </si>
+  <si>
+    <t>DOne</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.3 ACH </t>
+  </si>
+  <si>
+    <t>1.5 ACH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Base for HRV </t>
+  </si>
+  <si>
+    <t>Upgrade HRV</t>
+  </si>
+  <si>
+    <t>South+overhang</t>
+  </si>
+  <si>
+    <t>Triple hard coat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Base case - soft coat windows </t>
+  </si>
+  <si>
+    <t>Vs soft coat dbls</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gas cost </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Elec cost </t>
+  </si>
+  <si>
+    <t>Total savings ($/yr</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+  </numFmts>
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -308,13 +356,6 @@
       <b/>
       <u/>
       <sz val="42"/>
-      <color indexed="8"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="12"/>
       <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -397,7 +438,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -419,14 +460,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="1" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="1" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="1" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -804,10 +840,10 @@
   <dimension ref="A3:I41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="7" topLeftCell="C23" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="2" ySplit="7" topLeftCell="C18" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="B36" sqref="B36"/>
+      <selection pane="bottomRight" activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1072,7 +1108,7 @@
         <v>36</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>10</v>
+        <v>67</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
@@ -1088,7 +1124,7 @@
         <v>36</v>
       </c>
       <c r="G25" s="6" t="s">
-        <v>10</v>
+        <v>67</v>
       </c>
       <c r="H25" s="6"/>
       <c r="I25" s="6"/>
@@ -1120,9 +1156,11 @@
       <c r="E27" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="F27" s="6"/>
+      <c r="F27" s="6" t="s">
+        <v>19</v>
+      </c>
       <c r="G27" s="7" t="s">
-        <v>10</v>
+        <v>67</v>
       </c>
       <c r="H27" s="6"/>
       <c r="I27" s="6"/>
@@ -1179,10 +1217,10 @@
       </c>
       <c r="E30" s="5"/>
       <c r="F30" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="G30" s="5" t="s">
-        <v>10</v>
+        <v>67</v>
       </c>
       <c r="H30" s="5"/>
       <c r="I30" s="5" t="s">
@@ -1200,7 +1238,7 @@
       </c>
       <c r="F31" s="6"/>
       <c r="G31" s="6" t="s">
-        <v>10</v>
+        <v>86</v>
       </c>
       <c r="H31" s="6"/>
       <c r="I31" s="6"/>
@@ -1246,7 +1284,7 @@
         <v>19</v>
       </c>
       <c r="G34" s="6" t="s">
-        <v>10</v>
+        <v>67</v>
       </c>
       <c r="H34" s="6"/>
       <c r="I34" s="6"/>
@@ -1268,7 +1306,7 @@
         <v>19</v>
       </c>
       <c r="G35" s="6" t="s">
-        <v>10</v>
+        <v>67</v>
       </c>
       <c r="H35" s="6"/>
       <c r="I35" s="6"/>
@@ -1306,7 +1344,7 @@
         <v>2</v>
       </c>
       <c r="G37" s="6" t="s">
-        <v>10</v>
+        <v>67</v>
       </c>
       <c r="H37" s="6"/>
       <c r="I37" s="6"/>
@@ -1328,7 +1366,7 @@
         <v>19</v>
       </c>
       <c r="G38" s="6" t="s">
-        <v>10</v>
+        <v>67</v>
       </c>
       <c r="H38" s="7"/>
       <c r="I38" s="7"/>
@@ -1361,7 +1399,7 @@
         <v>2</v>
       </c>
       <c r="G40" s="5" t="s">
-        <v>10</v>
+        <v>67</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
@@ -1378,7 +1416,7 @@
         <v>2</v>
       </c>
       <c r="G41" s="6" t="s">
-        <v>10</v>
+        <v>67</v>
       </c>
       <c r="H41" s="6"/>
       <c r="I41" s="6"/>
@@ -1418,207 +1456,537 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C4:H13"/>
+  <dimension ref="C2:I29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.140625" style="1" customWidth="1"/>
     <col min="2" max="2" width="2.28515625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="27.28515625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="15.7109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="18.28515625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="19.7109375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="12.7109375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="15.140625" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="1"/>
+    <col min="3" max="3" width="22.85546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="15.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="18.28515625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="19.7109375" style="1" customWidth="1"/>
+    <col min="8" max="9" width="12.7109375" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="F2" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="G2" s="1">
+        <v>0.25580000000000003</v>
+      </c>
+    </row>
+    <row r="3" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="F3" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="G3" s="1">
+        <v>7.1830000000000005E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
-    </row>
-    <row r="5" spans="3:8" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+    </row>
+    <row r="5" spans="3:9" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C5" s="15" t="s">
         <v>68</v>
       </c>
-      <c r="D5" s="16" t="s">
+      <c r="D5" s="15"/>
+      <c r="E5" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="E5" s="16" t="s">
+      <c r="F5" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="F5" s="16" t="s">
+      <c r="G5" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="G5" s="16" t="s">
+      <c r="H5" s="16" t="s">
         <v>72</v>
       </c>
-      <c r="H5" s="23" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="I5" s="16" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="6" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C6" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="D6" s="18">
-        <v>12504.023999999999</v>
-      </c>
       <c r="E6" s="18">
-        <v>2341.5479999999998</v>
-      </c>
-      <c r="F6" s="17"/>
+        <v>12533</v>
+      </c>
+      <c r="F6" s="18">
+        <v>2401.6</v>
+      </c>
       <c r="G6" s="17"/>
-    </row>
-    <row r="7" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C7" s="19" t="s">
-        <v>77</v>
-      </c>
-      <c r="D7" s="20">
-        <v>12535.56</v>
-      </c>
-      <c r="E7" s="20">
-        <v>2404.62</v>
-      </c>
-      <c r="F7" s="21"/>
-      <c r="G7" s="21"/>
-    </row>
-    <row r="8" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="H6" s="17"/>
+      <c r="I6" s="17"/>
+    </row>
+    <row r="7" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C7" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="E7" s="18">
+        <v>12184.7346144</v>
+      </c>
+      <c r="F7" s="18">
+        <v>2660</v>
+      </c>
+      <c r="G7" s="17"/>
+      <c r="H7" s="17"/>
+      <c r="I7" s="17"/>
+    </row>
+    <row r="8" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C8" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="E8" s="18">
+        <v>12706.0191756</v>
+      </c>
+      <c r="F8" s="18">
+        <v>2413.9627765199998</v>
+      </c>
+      <c r="G8" s="17"/>
+      <c r="H8" s="17"/>
+      <c r="I8" s="17"/>
+    </row>
+    <row r="9" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C9" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E9" s="18">
+        <v>12530.283238800001</v>
+      </c>
+      <c r="F9" s="18">
+        <v>2383.40045052</v>
+      </c>
+      <c r="G9" s="18">
+        <f>$E$8-E9</f>
+        <v>175.73593679999976</v>
+      </c>
+      <c r="H9" s="18">
+        <f>$F$8-F9</f>
+        <v>30.562325999999757</v>
+      </c>
+      <c r="I9" s="18">
+        <f>H9*$G$2+G9*$G$3</f>
+        <v>20.440955331143922</v>
+      </c>
+    </row>
+    <row r="10" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C10" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D8" s="18">
-        <v>11967.12</v>
-      </c>
-      <c r="E8" s="18">
-        <f>E6</f>
-        <v>2341.5479999999998</v>
-      </c>
-      <c r="F8" s="18">
-        <f>$D$6-D8</f>
-        <v>536.90399999999863</v>
-      </c>
-      <c r="G8" s="18">
-        <f>$E$6-E8</f>
+      <c r="E10" s="18">
+        <v>11981.232018000001</v>
+      </c>
+      <c r="F10" s="18">
+        <v>2401.5066084</v>
+      </c>
+      <c r="G10" s="18">
+        <f>$E$6-E10</f>
+        <v>551.76798199999939</v>
+      </c>
+      <c r="H10" s="18">
+        <f>$F$6-F10</f>
+        <v>9.3391599999904429E-2</v>
+      </c>
+      <c r="I10" s="18">
+        <f t="shared" ref="I10:I25" si="0">H10*$G$2+G10*$G$3</f>
+        <v>39.657383718339929</v>
+      </c>
+    </row>
+    <row r="11" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C11" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="E11" s="18">
+        <v>8473.4748540000001</v>
+      </c>
+      <c r="F11" s="18">
+        <v>2786.28373044</v>
+      </c>
+      <c r="G11" s="18">
+        <f>$E$6-E11</f>
+        <v>4059.5251459999999</v>
+      </c>
+      <c r="H11" s="18">
+        <f>$F$6-F11</f>
+        <v>-384.68373044000009</v>
+      </c>
+      <c r="I11" s="18">
+        <f t="shared" si="0"/>
+        <v>193.19359299062796</v>
+      </c>
+    </row>
+    <row r="12" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C12" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E12" s="18">
+        <f>E6-4.60476*5*1000*1000/3600</f>
+        <v>6137.5</v>
+      </c>
+      <c r="F12" s="18">
+        <f>F6</f>
+        <v>2401.6</v>
+      </c>
+      <c r="G12" s="18">
+        <f>$E$6-E12</f>
+        <v>6395.5</v>
+      </c>
+      <c r="H12" s="18">
+        <f>$F$6-F12</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C9" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="D9" s="18">
-        <f>D6-4.60476*5*1000*1000/3600</f>
-        <v>6108.5239999999994</v>
-      </c>
-      <c r="E9" s="18">
-        <f>E6</f>
-        <v>2341.5479999999998</v>
-      </c>
-      <c r="F9" s="18">
-        <f>$D$6-D9</f>
-        <v>6395.5</v>
-      </c>
-      <c r="G9" s="18">
-        <f>$E$6-E9</f>
+      <c r="I12" s="18">
+        <f t="shared" si="0"/>
+        <v>459.38876500000003</v>
+      </c>
+    </row>
+    <row r="13" spans="3:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C13" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="E13" s="18">
+        <v>12528.606312</v>
+      </c>
+      <c r="F13" s="18">
+        <v>2383.1719721999998</v>
+      </c>
+      <c r="G13" s="18">
+        <f t="shared" ref="G13:G22" si="1">$E$6-E13</f>
+        <v>4.3936880000001111</v>
+      </c>
+      <c r="H13" s="18">
+        <f t="shared" ref="H13:H20" si="2">$F$6-F13</f>
+        <v>18.428027800000109</v>
+      </c>
+      <c r="I13" s="18">
+        <f t="shared" si="0"/>
+        <v>5.0294881202800363</v>
+      </c>
+    </row>
+    <row r="14" spans="3:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D14" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="E14" s="18">
+        <v>12491.614584000001</v>
+      </c>
+      <c r="F14" s="18">
+        <v>2045.5645856399999</v>
+      </c>
+      <c r="G14" s="18">
+        <f t="shared" ref="G14" si="3">$E$6-E14</f>
+        <v>41.385415999999168</v>
+      </c>
+      <c r="H14" s="18">
+        <f t="shared" ref="H14" si="4">$F$6-F14</f>
+        <v>356.03541436</v>
+      </c>
+      <c r="I14" s="18">
+        <f t="shared" si="0"/>
+        <v>94.046573424567953</v>
+      </c>
+    </row>
+    <row r="15" spans="3:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C15" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="E15" s="21">
+        <v>12498.241086</v>
+      </c>
+      <c r="F15" s="21">
+        <v>2299.3205864400002</v>
+      </c>
+      <c r="G15" s="18">
+        <f t="shared" ref="G15:G18" si="5">$E$6-E15</f>
+        <v>34.758914000000004</v>
+      </c>
+      <c r="H15" s="18">
+        <f t="shared" ref="H15:H18" si="6">$F$6-F15</f>
+        <v>102.27941355999974</v>
+      </c>
+      <c r="I15" s="18">
+        <f t="shared" si="0"/>
+        <v>28.659806781267939</v>
+      </c>
+    </row>
+    <row r="16" spans="3:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C16" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="E16" s="18">
+        <v>12490.7047704</v>
+      </c>
+      <c r="F16" s="18">
+        <v>2196.0385308</v>
+      </c>
+      <c r="G16" s="18">
+        <f t="shared" si="5"/>
+        <v>42.295229600000312</v>
+      </c>
+      <c r="H16" s="18">
+        <f t="shared" si="6"/>
+        <v>205.56146919999992</v>
+      </c>
+      <c r="I16" s="18">
+        <f t="shared" si="0"/>
+        <v>55.62069016352801</v>
+      </c>
+    </row>
+    <row r="17" spans="3:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D17" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="E17" s="21">
+        <v>12482.547984000001</v>
+      </c>
+      <c r="F17" s="21">
+        <v>2136.9822462000002</v>
+      </c>
+      <c r="G17" s="18">
+        <f t="shared" si="5"/>
+        <v>50.452015999999276</v>
+      </c>
+      <c r="H17" s="18">
+        <f t="shared" si="6"/>
+        <v>264.61775379999972</v>
+      </c>
+      <c r="I17" s="18">
+        <f t="shared" si="0"/>
+        <v>71.313189731319881</v>
+      </c>
+    </row>
+    <row r="18" spans="3:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D18" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="E18" s="18">
+        <v>12477.486456000001</v>
+      </c>
+      <c r="F18" s="18">
+        <v>2096.0567175599999</v>
+      </c>
+      <c r="G18" s="18">
+        <f t="shared" si="5"/>
+        <v>55.513543999999456</v>
+      </c>
+      <c r="H18" s="18">
+        <f t="shared" si="6"/>
+        <v>305.54328243999998</v>
+      </c>
+      <c r="I18" s="18">
+        <f t="shared" si="0"/>
+        <v>82.145509513671954</v>
+      </c>
+    </row>
+    <row r="19" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C19" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E19" s="18">
+        <v>26170.346699999998</v>
+      </c>
+      <c r="F19" s="18">
         <v>0</v>
       </c>
-      <c r="H9" s="19"/>
-    </row>
-    <row r="10" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C10" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="D10" s="18">
-        <v>12472.487999999999</v>
-      </c>
-      <c r="E10" s="18">
-        <v>2144.4479999999999</v>
-      </c>
-      <c r="F10" s="18">
-        <f>IF(D10&gt;0,$D$7-D10,"")</f>
-        <v>63.072000000000116</v>
-      </c>
-      <c r="G10" s="18">
-        <f>IF(E10&gt;0,$E$7-E10,"")</f>
-        <v>260.17200000000003</v>
-      </c>
-      <c r="H10" s="19" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="11" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C11" s="1" t="s">
+      <c r="G19" s="18">
+        <f t="shared" si="1"/>
+        <v>-13637.346699999998</v>
+      </c>
+      <c r="H19" s="18">
+        <f t="shared" si="2"/>
+        <v>2401.6</v>
+      </c>
+      <c r="I19" s="18">
+        <f t="shared" si="0"/>
+        <v>-365.24133346099995</v>
+      </c>
+    </row>
+    <row r="20" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C20" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="D11" s="18">
-        <v>12472.487999999999</v>
-      </c>
-      <c r="E11" s="18">
-        <v>2144.4479999999999</v>
-      </c>
-      <c r="F11" s="18">
-        <f>IF(D11&gt;0,$D$7-D11, "")</f>
-        <v>63.072000000000116</v>
-      </c>
-      <c r="G11" s="18">
-        <f>IF(E11&gt;0,$E$7-E11,"")</f>
-        <v>260.17200000000003</v>
-      </c>
-      <c r="H11" s="19" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="12" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C12" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="D12" s="18">
-        <v>12535.56</v>
-      </c>
-      <c r="E12" s="18">
-        <v>2373.0839999999998</v>
-      </c>
-      <c r="F12" s="18">
-        <f t="shared" ref="F12:F13" si="0">IF(D12&gt;0,$D$7-D12, "")</f>
-        <v>0</v>
-      </c>
-      <c r="G12" s="18">
-        <f t="shared" ref="G12:G13" si="1">IF(E12&gt;0,$E$7-E12,"")</f>
-        <v>31.536000000000058</v>
-      </c>
-      <c r="H12" s="19" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="13" spans="3:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C13" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="D13" s="22">
-        <v>12504.023999999999</v>
-      </c>
-      <c r="E13" s="22">
-        <v>2310.0120000000002</v>
-      </c>
-      <c r="F13" s="22">
+      <c r="D20" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E20" s="18">
+        <v>12429.174880799999</v>
+      </c>
+      <c r="F20" s="18">
+        <v>2268.2624356800002</v>
+      </c>
+      <c r="G20" s="18">
+        <f t="shared" si="1"/>
+        <v>103.8251192000007</v>
+      </c>
+      <c r="H20" s="18">
+        <f t="shared" si="2"/>
+        <v>133.33756431999973</v>
+      </c>
+      <c r="I20" s="20">
         <f t="shared" si="0"/>
-        <v>31.536000000000058</v>
-      </c>
-      <c r="G13" s="22">
+        <v>41.565507265191982</v>
+      </c>
+    </row>
+    <row r="21" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="D21" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="E21" s="18">
+        <v>12429.174880799999</v>
+      </c>
+      <c r="F21" s="18">
+        <v>2268.2624356800002</v>
+      </c>
+      <c r="G21" s="18">
+        <f>$E$7-E21</f>
+        <v>-244.44026639999902</v>
+      </c>
+      <c r="H21" s="18">
+        <f>$F$7-F21</f>
+        <v>391.73756431999982</v>
+      </c>
+      <c r="I21" s="18">
+        <f t="shared" si="0"/>
+        <v>82.648324617544034</v>
+      </c>
+    </row>
+    <row r="22" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C22" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E22" s="18">
+        <v>12551.236545600001</v>
+      </c>
+      <c r="F22" s="18">
+        <v>2234.19819456</v>
+      </c>
+      <c r="G22" s="18">
         <f t="shared" si="1"/>
-        <v>94.60799999999972</v>
-      </c>
-      <c r="H13" s="24" t="s">
-        <v>81</v>
-      </c>
+        <v>-18.236545600000682</v>
+      </c>
+      <c r="H22" s="18">
+        <f t="shared" ref="H22:H24" si="7">$F$6-F22</f>
+        <v>167.40180543999986</v>
+      </c>
+      <c r="I22" s="18">
+        <f t="shared" si="0"/>
+        <v>41.511450761103916</v>
+      </c>
+    </row>
+    <row r="23" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="D23" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="E23" s="18">
+        <v>12430.8857088</v>
+      </c>
+      <c r="F23" s="18">
+        <v>2246.8841812800001</v>
+      </c>
+      <c r="G23" s="18">
+        <f>$E$6-E23</f>
+        <v>102.11429119999957</v>
+      </c>
+      <c r="H23" s="18">
+        <f t="shared" ref="H23" si="8">$F$6-F23</f>
+        <v>154.71581871999979</v>
+      </c>
+      <c r="I23" s="18">
+        <f t="shared" si="0"/>
+        <v>46.911175965471919</v>
+      </c>
+    </row>
+    <row r="24" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="D24" s="1" t="str">
+        <f>"+Extra windows"</f>
+        <v>+Extra windows</v>
+      </c>
+      <c r="E24" s="18">
+        <v>12750.7805856</v>
+      </c>
+      <c r="F24" s="18">
+        <v>2183.4012671999999</v>
+      </c>
+      <c r="G24" s="18">
+        <f t="shared" ref="G24" si="9">$E$6-E24</f>
+        <v>-217.78058559999954</v>
+      </c>
+      <c r="H24" s="18">
+        <f t="shared" si="7"/>
+        <v>218.19873280000002</v>
+      </c>
+      <c r="I24" s="18">
+        <f t="shared" si="0"/>
+        <v>40.17205638659204</v>
+      </c>
+    </row>
+    <row r="25" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C25" s="2"/>
+      <c r="D25" s="2" t="str">
+        <f>"+Overhang &amp;drywall"</f>
+        <v>+Overhang &amp;drywall</v>
+      </c>
+      <c r="E25" s="19">
+        <v>12620.041790400001</v>
+      </c>
+      <c r="F25" s="19">
+        <v>2187.2076624000001</v>
+      </c>
+      <c r="G25" s="19">
+        <f t="shared" ref="G25" si="10">$E$6-E25</f>
+        <v>-87.041790400000536</v>
+      </c>
+      <c r="H25" s="19">
+        <f t="shared" ref="H25" si="11">$F$6-F25</f>
+        <v>214.39233759999979</v>
+      </c>
+      <c r="I25" s="19">
+        <f t="shared" si="0"/>
+        <v>48.589348153647919</v>
+      </c>
+    </row>
+    <row r="26" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="E26" s="20"/>
+      <c r="F26" s="20"/>
+      <c r="I26" s="18"/>
+    </row>
+    <row r="27" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="E27" s="20"/>
+      <c r="F27" s="20"/>
+    </row>
+    <row r="28" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="E28" s="20"/>
+      <c r="F28" s="20"/>
+    </row>
+    <row r="29" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="E29" s="20"/>
+      <c r="F29" s="20"/>
     </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>

</xml_diff>